<commit_message>
Updated code to include control signal stats
</commit_message>
<xml_diff>
--- a/PythonSourceCode/AirHeaterFMUwithMPC/datafiles/describeExport.xlsx
+++ b/PythonSourceCode/AirHeaterFMUwithMPC/datafiles/describeExport.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,10 +446,20 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>controlSignalPython</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>controlSignalFMU</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>outputTemperaturePython</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>outputTemperatureFMU</t>
         </is>
@@ -473,6 +483,12 @@
       <c r="E2" t="n">
         <v>2921</v>
       </c>
+      <c r="F2" t="n">
+        <v>2921</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2921</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -487,9 +503,15 @@
         <v>30.51386511468675</v>
       </c>
       <c r="D3" t="n">
+        <v>0.696351587164061</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.6961559566308066</v>
+      </c>
+      <c r="F3" t="n">
         <v>30.25852714114286</v>
       </c>
-      <c r="E3" t="n">
+      <c r="G3" t="n">
         <v>30.25595573643138</v>
       </c>
     </row>
@@ -506,9 +528,15 @@
         <v>0.9633447125636713</v>
       </c>
       <c r="D4" t="n">
+        <v>0.4168086750774854</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.4170013826581315</v>
+      </c>
+      <c r="F4" t="n">
         <v>0.6917165266705572</v>
       </c>
-      <c r="E4" t="n">
+      <c r="G4" t="n">
         <v>0.6879256989230766</v>
       </c>
     </row>
@@ -525,9 +553,15 @@
         <v>28.5</v>
       </c>
       <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
         <v>28</v>
       </c>
-      <c r="E5" t="n">
+      <c r="G5" t="n">
         <v>28</v>
       </c>
     </row>
@@ -544,9 +578,15 @@
         <v>30.07536647726965</v>
       </c>
       <c r="D6" t="n">
+        <v>0.6497365006255256</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.6497365006255256</v>
+      </c>
+      <c r="F6" t="n">
         <v>30.17602260595553</v>
       </c>
-      <c r="E6" t="n">
+      <c r="G6" t="n">
         <v>30.17559522630141</v>
       </c>
     </row>
@@ -563,9 +603,15 @@
         <v>32</v>
       </c>
       <c r="D7" t="n">
+        <v>2.174568593007422</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2.174568593007422</v>
+      </c>
+      <c r="F7" t="n">
         <v>31.00450136605604</v>
       </c>
-      <c r="E7" t="n">
+      <c r="G7" t="n">
         <v>31.00360907210886</v>
       </c>
     </row>

</xml_diff>